<commit_message>
Moving to producer consumer pattern for generating data for all the companies
</commit_message>
<xml_diff>
--- a/Data/demo.xlsx
+++ b/Data/demo.xlsx
@@ -1,20 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="24816"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="20" windowWidth="16100" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="176">
   <si>
     <t>No</t>
   </si>
@@ -542,88 +547,13 @@
   </si>
   <si>
     <t>Jack Prim</t>
-  </si>
-  <si>
-    <t>Bazaarvoice</t>
-  </si>
-  <si>
-    <t>Austin, TX</t>
-  </si>
-  <si>
-    <t>Gene Austin</t>
-  </si>
-  <si>
-    <t>Lithium Technologies</t>
-  </si>
-  <si>
-    <t>Rob Tarkoff</t>
-  </si>
-  <si>
-    <t>MINDBODY</t>
-  </si>
-  <si>
-    <t>San Luis Obispo, CA</t>
-  </si>
-  <si>
-    <t>Rick Stollmeyer</t>
-  </si>
-  <si>
-    <t>Cvent</t>
-  </si>
-  <si>
-    <t>Mc Lean, VA</t>
-  </si>
-  <si>
-    <t>Reggie Aggarwal</t>
-  </si>
-  <si>
-    <t>Alltel</t>
-  </si>
-  <si>
-    <t>Little Rock, AR</t>
-  </si>
-  <si>
-    <t>Scott T. Ford</t>
-  </si>
-  <si>
-    <t>Fusion-io</t>
-  </si>
-  <si>
-    <t>Salt Lake City, UT</t>
-  </si>
-  <si>
-    <t>Shane Robison</t>
-  </si>
-  <si>
-    <t>Hubspot</t>
-  </si>
-  <si>
-    <t>Brian Halligan</t>
-  </si>
-  <si>
-    <t>ExactTarget Marketing Cloud</t>
-  </si>
-  <si>
-    <t>Scott McCorkle</t>
-  </si>
-  <si>
-    <t>100</t>
-  </si>
-  <si>
-    <t>Workday</t>
-  </si>
-  <si>
-    <t>Pleasanton, CA</t>
-  </si>
-  <si>
-    <t>Aneel Bhusri</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -635,6 +565,22 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -657,14 +603,30 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="9">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -956,12 +918,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F59"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="A51" sqref="A51:G67"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="2" max="2" width="28.6640625" customWidth="1"/>
+    <col min="4" max="4" width="44.6640625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
@@ -1963,187 +1931,13 @@
         <v>68</v>
       </c>
     </row>
-    <row r="51" spans="1:6">
-      <c r="A51">
-        <v>50</v>
-      </c>
-      <c r="B51" t="s">
-        <v>176</v>
-      </c>
-      <c r="C51" t="s">
-        <v>7</v>
-      </c>
-      <c r="D51" t="s">
-        <v>177</v>
-      </c>
-      <c r="E51" t="s">
-        <v>178</v>
-      </c>
-      <c r="F51" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6">
-      <c r="A52">
-        <v>51</v>
-      </c>
-      <c r="B52" t="s">
-        <v>179</v>
-      </c>
-      <c r="C52" t="s">
-        <v>80</v>
-      </c>
-      <c r="D52" t="s">
-        <v>35</v>
-      </c>
-      <c r="E52" t="s">
-        <v>180</v>
-      </c>
-      <c r="F52" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6">
-      <c r="A53">
-        <v>52</v>
-      </c>
-      <c r="B53" t="s">
-        <v>181</v>
-      </c>
-      <c r="C53" t="s">
-        <v>77</v>
-      </c>
-      <c r="D53" t="s">
-        <v>182</v>
-      </c>
-      <c r="E53" t="s">
-        <v>183</v>
-      </c>
-      <c r="F53" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6">
-      <c r="A54">
-        <v>53</v>
-      </c>
-      <c r="B54" t="s">
-        <v>184</v>
-      </c>
-      <c r="C54" t="s">
-        <v>7</v>
-      </c>
-      <c r="D54" t="s">
-        <v>185</v>
-      </c>
-      <c r="E54" t="s">
-        <v>186</v>
-      </c>
-      <c r="F54" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6">
-      <c r="A55">
-        <v>54</v>
-      </c>
-      <c r="B55" t="s">
-        <v>187</v>
-      </c>
-      <c r="C55" t="s">
-        <v>80</v>
-      </c>
-      <c r="D55" t="s">
-        <v>188</v>
-      </c>
-      <c r="E55" t="s">
-        <v>189</v>
-      </c>
-      <c r="F55" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6">
-      <c r="A56">
-        <v>55</v>
-      </c>
-      <c r="B56" t="s">
-        <v>190</v>
-      </c>
-      <c r="C56" t="s">
-        <v>63</v>
-      </c>
-      <c r="D56" t="s">
-        <v>191</v>
-      </c>
-      <c r="E56" t="s">
-        <v>192</v>
-      </c>
-      <c r="F56" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6">
-      <c r="A57">
-        <v>56</v>
-      </c>
-      <c r="B57" t="s">
-        <v>193</v>
-      </c>
-      <c r="C57" t="s">
-        <v>63</v>
-      </c>
-      <c r="D57" t="s">
-        <v>159</v>
-      </c>
-      <c r="E57" t="s">
-        <v>194</v>
-      </c>
-      <c r="F57" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6">
-      <c r="A58">
-        <v>57</v>
-      </c>
-      <c r="B58" t="s">
-        <v>195</v>
-      </c>
-      <c r="C58" t="s">
-        <v>80</v>
-      </c>
-      <c r="D58" t="s">
-        <v>92</v>
-      </c>
-      <c r="E58" t="s">
-        <v>196</v>
-      </c>
-      <c r="F58" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6">
-      <c r="A59">
-        <v>58</v>
-      </c>
-      <c r="B59" t="s">
-        <v>198</v>
-      </c>
-      <c r="C59" t="s">
-        <v>63</v>
-      </c>
-      <c r="D59" t="s">
-        <v>199</v>
-      </c>
-      <c r="E59" t="s">
-        <v>200</v>
-      </c>
-      <c r="F59" t="s">
-        <v>52</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>